<commit_message>
Update Service DH efficieny
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SRV_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_SRV_NewTechs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B6D636-40CD-440E-8DCF-46D1103F30EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA94D01-D6B8-4C62-802D-ADD0D4F3C935}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6750" yWindow="1305" windowWidth="16470" windowHeight="7470" tabRatio="789" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="789" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="78" r:id="rId1"/>
@@ -13892,10 +13892,6 @@
     <xf numFmtId="0" fontId="54" fillId="7" borderId="0" xfId="117" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -13905,6 +13901,10 @@
     <xf numFmtId="0" fontId="26" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -18809,46 +18809,46 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="446" t="s">
+      <c r="A3" s="442" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="446" t="s">
+      <c r="B3" s="442" t="s">
         <v>159</v>
       </c>
-      <c r="C3" s="446" t="s">
+      <c r="C3" s="442" t="s">
         <v>160</v>
       </c>
-      <c r="D3" s="448" t="s">
+      <c r="D3" s="444" t="s">
         <v>161</v>
       </c>
-      <c r="E3" s="448"/>
-      <c r="F3" s="446" t="s">
+      <c r="E3" s="444"/>
+      <c r="F3" s="442" t="s">
         <v>162</v>
       </c>
-      <c r="G3" s="446" t="s">
+      <c r="G3" s="442" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="446" t="s">
+      <c r="H3" s="442" t="s">
         <v>163</v>
       </c>
-      <c r="I3" s="446" t="s">
+      <c r="I3" s="442" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="447"/>
-      <c r="B4" s="447"/>
-      <c r="C4" s="447"/>
+      <c r="A4" s="443"/>
+      <c r="B4" s="443"/>
+      <c r="C4" s="443"/>
       <c r="D4" s="72" t="s">
         <v>165</v>
       </c>
       <c r="E4" s="72" t="s">
         <v>166</v>
       </c>
-      <c r="F4" s="447"/>
-      <c r="G4" s="447"/>
-      <c r="H4" s="447"/>
-      <c r="I4" s="447"/>
+      <c r="F4" s="443"/>
+      <c r="G4" s="443"/>
+      <c r="H4" s="443"/>
+      <c r="I4" s="443"/>
     </row>
     <row r="5" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
@@ -18934,18 +18934,18 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="189"/>
-      <c r="B11" s="442" t="str">
+      <c r="B11" s="445" t="str">
         <f>"Data summary table with data from "&amp;A5</f>
         <v>Data summary table with data from S1</v>
       </c>
-      <c r="C11" s="443"/>
+      <c r="C11" s="446"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
-      <c r="B12" s="444" t="s">
+      <c r="B12" s="447" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="445"/>
+      <c r="C12" s="448"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="24"/>
@@ -19315,16 +19315,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="G3:G4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="G3:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -20106,11 +20106,11 @@
   <dimension ref="A1:AY122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="X4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B21" sqref="B21"/>
       <selection pane="topRight" activeCell="B21" sqref="B21"/>
       <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
-      <selection pane="bottomRight" activeCell="AC18" sqref="AC18"/>
+      <selection pane="bottomRight" activeCell="P29" sqref="P29:T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23178,24 +23178,19 @@
       <c r="N29" s="353"/>
       <c r="O29" s="353"/>
       <c r="P29" s="353">
-        <f>F29</f>
-        <v>1.4</v>
+        <v>1.29</v>
       </c>
       <c r="Q29" s="353">
-        <f t="shared" ref="Q29:T29" si="16">G29</f>
-        <v>1.4</v>
+        <v>1.29</v>
       </c>
       <c r="R29" s="353">
-        <f t="shared" si="16"/>
-        <v>1.4</v>
+        <v>1.29</v>
       </c>
       <c r="S29" s="353">
-        <f t="shared" si="16"/>
-        <v>1.4</v>
+        <v>1.29</v>
       </c>
       <c r="T29" s="353">
-        <f t="shared" si="16"/>
-        <v>1.4</v>
+        <v>1.29</v>
       </c>
       <c r="U29" s="354">
         <f>'JRC data'!AX62</f>
@@ -23363,31 +23358,31 @@
       <c r="Z31" s="349"/>
       <c r="AA31" s="349"/>
       <c r="AB31" s="349">
-        <f t="shared" ref="AB31:AH31" si="17">AB16</f>
+        <f t="shared" ref="AB31:AH31" si="16">AB16</f>
         <v>665</v>
       </c>
       <c r="AC31" s="349">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>665</v>
       </c>
       <c r="AD31" s="349">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>665</v>
       </c>
       <c r="AE31" s="349">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>665</v>
       </c>
       <c r="AF31" s="349">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>665</v>
       </c>
       <c r="AG31" s="350">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>10</v>
       </c>
       <c r="AH31" s="351">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="AI31" s="34"/>
@@ -23563,51 +23558,51 @@
       </c>
       <c r="V33" s="348"/>
       <c r="W33" s="349">
-        <f t="shared" ref="W33:AH33" si="18">W7</f>
+        <f t="shared" ref="W33:AH33" si="17">W7</f>
         <v>22500</v>
       </c>
       <c r="X33" s="349">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>20000</v>
       </c>
       <c r="Y33" s="349">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>17500</v>
       </c>
       <c r="Z33" s="349">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>17500</v>
       </c>
       <c r="AA33" s="349">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>17500</v>
       </c>
       <c r="AB33" s="349">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>58.441558441558442</v>
       </c>
       <c r="AC33" s="349">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>51.948051948051948</v>
       </c>
       <c r="AD33" s="349">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>45.454545454545453</v>
       </c>
       <c r="AE33" s="349">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>45.454545454545453</v>
       </c>
       <c r="AF33" s="349">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>45.454545454545453</v>
       </c>
       <c r="AG33" s="350">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
       <c r="AH33" s="351">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
       <c r="AI33" s="34"/>
@@ -23649,76 +23644,76 @@
       <c r="N34" s="347"/>
       <c r="O34" s="347"/>
       <c r="P34" s="347">
-        <f t="shared" ref="P34:U34" si="19">P14</f>
+        <f t="shared" ref="P34:U34" si="18">P14</f>
         <v>0.7</v>
       </c>
       <c r="Q34" s="347">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.71647058823529397</v>
       </c>
       <c r="R34" s="347">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.74941176470588233</v>
       </c>
       <c r="S34" s="347">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.78235294117647058</v>
       </c>
       <c r="T34" s="347">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.78235294117647058</v>
       </c>
       <c r="U34" s="348">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>20</v>
       </c>
       <c r="V34" s="348"/>
       <c r="W34" s="349">
-        <f t="shared" ref="W34:AH34" si="20">W13</f>
+        <f t="shared" ref="W34:AH34" si="19">W13</f>
         <v>108500</v>
       </c>
       <c r="X34" s="349">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>108500</v>
       </c>
       <c r="Y34" s="349">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>112000</v>
       </c>
       <c r="Z34" s="349">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>112000</v>
       </c>
       <c r="AA34" s="349">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>112000</v>
       </c>
       <c r="AB34" s="349">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>197.27272727272728</v>
       </c>
       <c r="AC34" s="349">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>197.27272727272728</v>
       </c>
       <c r="AD34" s="349">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>203.63636363636363</v>
       </c>
       <c r="AE34" s="349">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>203.63636363636363</v>
       </c>
       <c r="AF34" s="349">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>203.63636363636363</v>
       </c>
       <c r="AG34" s="350">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>5.7272727272727274E-2</v>
       </c>
       <c r="AH34" s="351">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AI34" s="34"/>
@@ -23760,76 +23755,76 @@
       <c r="N35" s="353"/>
       <c r="O35" s="353"/>
       <c r="P35" s="353">
-        <f t="shared" ref="P35:U35" si="21">P12</f>
+        <f t="shared" ref="P35:U35" si="20">P12</f>
         <v>0.7</v>
       </c>
       <c r="Q35" s="353">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>0.7</v>
       </c>
       <c r="R35" s="353">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>0.7</v>
       </c>
       <c r="S35" s="353">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>0.7</v>
       </c>
       <c r="T35" s="353">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>0.7</v>
       </c>
       <c r="U35" s="354">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>25</v>
       </c>
       <c r="V35" s="354"/>
       <c r="W35" s="355">
-        <f t="shared" ref="W35:AH35" si="22">W33</f>
+        <f t="shared" ref="W35:AH35" si="21">W33</f>
         <v>22500</v>
       </c>
       <c r="X35" s="355">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>20000</v>
       </c>
       <c r="Y35" s="355">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>17500</v>
       </c>
       <c r="Z35" s="355">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>17500</v>
       </c>
       <c r="AA35" s="355">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>17500</v>
       </c>
       <c r="AB35" s="355">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>58.441558441558442</v>
       </c>
       <c r="AC35" s="355">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>51.948051948051948</v>
       </c>
       <c r="AD35" s="355">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>45.454545454545453</v>
       </c>
       <c r="AE35" s="355">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>45.454545454545453</v>
       </c>
       <c r="AF35" s="355">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>45.454545454545453</v>
       </c>
       <c r="AG35" s="356">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>4</v>
       </c>
       <c r="AH35" s="357">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="AI35" s="37"/>
@@ -23944,51 +23939,51 @@
       </c>
       <c r="V37" s="371"/>
       <c r="W37" s="349">
-        <f t="shared" ref="W37:AH37" si="23">W18</f>
+        <f t="shared" ref="W37:AH37" si="22">W18</f>
         <v>27140.2</v>
       </c>
       <c r="X37" s="349">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>25783.19</v>
       </c>
       <c r="Y37" s="349">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>23340.571999999996</v>
       </c>
       <c r="Z37" s="349">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>22254.963999999996</v>
       </c>
       <c r="AA37" s="349">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>22254.963999999996</v>
       </c>
       <c r="AB37" s="349">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>426.06279434850865</v>
       </c>
       <c r="AC37" s="349">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>404.75965463108315</v>
       </c>
       <c r="AD37" s="349">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>366.41400313971735</v>
       </c>
       <c r="AE37" s="349">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>349.37149136577699</v>
       </c>
       <c r="AF37" s="349">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>349.37149136577699</v>
       </c>
       <c r="AG37" s="350">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>10.204081632653061</v>
       </c>
       <c r="AH37" s="351">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AI37" s="34"/>
@@ -24695,7 +24690,7 @@
       <c r="AO47" s="211"/>
       <c r="AP47" s="172"/>
       <c r="AQ47" s="224" t="str">
-        <f t="shared" ref="AQ47:AQ80" si="24">IF(LEFT(A47)="*",A47,"PRE")</f>
+        <f t="shared" ref="AQ47:AQ80" si="23">IF(LEFT(A47)="*",A47,"PRE")</f>
         <v>*Boilers</v>
       </c>
       <c r="AR47" s="280" t="str">
@@ -24703,19 +24698,19 @@
         <v/>
       </c>
       <c r="AS47" s="224" t="str">
-        <f t="shared" ref="AS47:AT80" si="25">IF(LEFT($A47)="*","",A47)</f>
+        <f t="shared" ref="AS47:AT80" si="24">IF(LEFT($A47)="*","",A47)</f>
         <v/>
       </c>
       <c r="AT47" s="224" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AU47" s="224" t="str">
-        <f t="shared" ref="AU47:AU81" si="26">IF(LEFT($A47)="*","","PJ")</f>
+        <f t="shared" ref="AU47:AU81" si="25">IF(LEFT($A47)="*","","PJ")</f>
         <v/>
       </c>
       <c r="AV47" s="224" t="str">
-        <f t="shared" ref="AV47:AV81" si="27">IF(LEFT($A47)="*","","GW")</f>
+        <f t="shared" ref="AV47:AV81" si="26">IF(LEFT($A47)="*","","GW")</f>
         <v/>
       </c>
       <c r="AW47" s="42" t="str">
@@ -24724,7 +24719,7 @@
       </c>
       <c r="AX47" s="224"/>
       <c r="AY47" s="224" t="str">
-        <f t="shared" ref="AY47" si="28">IF($AS47="","","YES")</f>
+        <f t="shared" ref="AY47" si="27">IF($AS47="","","YES")</f>
         <v/>
       </c>
     </row>
@@ -24855,7 +24850,7 @@
         <v/>
       </c>
       <c r="AK48" s="68">
-        <f t="shared" ref="AK48:AK57" si="29">IF($A48="*","",31.536)</f>
+        <f t="shared" ref="AK48:AK57" si="28">IF($A48="*","",31.536)</f>
         <v>31.536000000000001</v>
       </c>
       <c r="AL48" s="40"/>
@@ -24867,7 +24862,7 @@
       <c r="AO48" s="211"/>
       <c r="AP48" s="172"/>
       <c r="AQ48" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR48" s="280" t="str">
@@ -24875,19 +24870,19 @@
         <v>IE,National</v>
       </c>
       <c r="AS48" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS_OIL_N1</v>
+      </c>
+      <c r="AT48" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Oil boiler condensing_SH</v>
+      </c>
+      <c r="AU48" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS_OIL_N1</v>
-      </c>
-      <c r="AT48" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Oil boiler condensing_SH</v>
-      </c>
-      <c r="AU48" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV48" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV48" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY48" s="42" t="str">
@@ -25022,19 +25017,19 @@
         <v/>
       </c>
       <c r="AK49" s="68">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL49" s="40"/>
       <c r="AM49" s="81">
-        <f t="shared" ref="AM49:AM81" si="30">IF($A49="*","",2019)</f>
+        <f t="shared" ref="AM49:AM81" si="29">IF($A49="*","",2019)</f>
         <v>2019</v>
       </c>
       <c r="AN49" s="211"/>
       <c r="AO49" s="211"/>
       <c r="AP49" s="172"/>
       <c r="AQ49" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR49" s="42" t="str">
@@ -25042,23 +25037,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS49" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS_OIL_N2</v>
+      </c>
+      <c r="AT49" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Oil boiler condensing_SH-WH</v>
+      </c>
+      <c r="AU49" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS_OIL_N2</v>
-      </c>
-      <c r="AT49" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Oil boiler condensing_SH-WH</v>
-      </c>
-      <c r="AU49" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV49" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV49" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY49" s="42" t="str">
-        <f t="shared" ref="AY49:AY81" si="31">IF($AS49="","","YES")</f>
+        <f t="shared" ref="AY49:AY81" si="30">IF($AS49="","","YES")</f>
         <v>YES</v>
       </c>
     </row>
@@ -25189,19 +25184,19 @@
         <v/>
       </c>
       <c r="AK50" s="68">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL50" s="40"/>
       <c r="AM50" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN50" s="211"/>
       <c r="AO50" s="211"/>
       <c r="AP50" s="172"/>
       <c r="AQ50" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR50" s="42" t="str">
@@ -25209,23 +25204,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS50" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS_GAS_N1</v>
+      </c>
+      <c r="AT50" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Gas boiler condensing_SH</v>
+      </c>
+      <c r="AU50" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS_GAS_N1</v>
-      </c>
-      <c r="AT50" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Gas boiler condensing_SH</v>
-      </c>
-      <c r="AU50" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV50" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV50" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY50" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -25356,19 +25351,19 @@
         <v/>
       </c>
       <c r="AK51" s="68">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL51" s="40"/>
       <c r="AM51" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN51" s="211"/>
       <c r="AO51" s="211"/>
       <c r="AP51" s="172"/>
       <c r="AQ51" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR51" s="42" t="str">
@@ -25376,23 +25371,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS51" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS_GAS_N2</v>
+      </c>
+      <c r="AT51" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">Commercial Services - Gas boiler condensing_SH-WH </v>
+      </c>
+      <c r="AU51" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS_GAS_N2</v>
-      </c>
-      <c r="AT51" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v xml:space="preserve">Commercial Services - Gas boiler condensing_SH-WH </v>
-      </c>
-      <c r="AU51" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV51" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV51" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY51" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -25523,19 +25518,19 @@
         <v/>
       </c>
       <c r="AK52" s="68">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL52" s="40"/>
       <c r="AM52" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN52" s="211"/>
       <c r="AO52" s="211"/>
       <c r="AP52" s="172"/>
       <c r="AQ52" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR52" s="42" t="str">
@@ -25543,23 +25538,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS52" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS_GAS_N3</v>
+      </c>
+      <c r="AT52" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">Commercial Services - Gas boiler condensing + Solar thermal_SH-WH </v>
+      </c>
+      <c r="AU52" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS_GAS_N3</v>
-      </c>
-      <c r="AT52" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v xml:space="preserve">Commercial Services - Gas boiler condensing + Solar thermal_SH-WH </v>
-      </c>
-      <c r="AU52" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV52" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV52" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY52" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -25690,19 +25685,19 @@
         <v>0.51127819548872178</v>
       </c>
       <c r="AK53" s="68">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL53" s="40"/>
       <c r="AM53" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN53" s="211"/>
       <c r="AO53" s="211"/>
       <c r="AP53" s="172"/>
       <c r="AQ53" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR53" s="42" t="str">
@@ -25710,23 +25705,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS53" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS-GAS_N4</v>
+      </c>
+      <c r="AT53" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v xml:space="preserve">Commercial Services - Gas boiler condensing + Wood stove_SH-WH </v>
+      </c>
+      <c r="AU53" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS-GAS_N4</v>
-      </c>
-      <c r="AT53" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v xml:space="preserve">Commercial Services - Gas boiler condensing + Wood stove_SH-WH </v>
-      </c>
-      <c r="AU53" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV53" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV53" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY53" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -25857,19 +25852,19 @@
         <v/>
       </c>
       <c r="AK54" s="68">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL54" s="84"/>
       <c r="AM54" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN54" s="211"/>
       <c r="AO54" s="211"/>
       <c r="AP54" s="172"/>
       <c r="AQ54" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR54" s="42" t="str">
@@ -25877,23 +25872,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS54" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS_LPG_N1</v>
+      </c>
+      <c r="AT54" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - LPG boiler condensing_SH</v>
+      </c>
+      <c r="AU54" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS_LPG_N1</v>
-      </c>
-      <c r="AT54" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - LPG boiler condensing_SH</v>
-      </c>
-      <c r="AU54" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV54" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV54" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY54" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -26024,19 +26019,19 @@
         <v/>
       </c>
       <c r="AK55" s="68">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL55" s="84"/>
       <c r="AM55" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN55" s="211"/>
       <c r="AO55" s="211"/>
       <c r="AP55" s="172"/>
       <c r="AQ55" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR55" s="42" t="str">
@@ -26044,23 +26039,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS55" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS_LPG_N2</v>
+      </c>
+      <c r="AT55" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - LPG boiler condensing_SH-WH</v>
+      </c>
+      <c r="AU55" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS_LPG_N2</v>
-      </c>
-      <c r="AT55" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - LPG boiler condensing_SH-WH</v>
-      </c>
-      <c r="AU55" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV55" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV55" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY55" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -26192,19 +26187,19 @@
         <v/>
       </c>
       <c r="AK56" s="68">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL56" s="40"/>
       <c r="AM56" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN56" s="211"/>
       <c r="AO56" s="211"/>
       <c r="AP56" s="172"/>
       <c r="AQ56" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR56" s="42" t="str">
@@ -26212,23 +26207,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS56" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS_BIO_N1</v>
+      </c>
+      <c r="AT56" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Biomass boiler_SH</v>
+      </c>
+      <c r="AU56" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS_BIO_N1</v>
-      </c>
-      <c r="AT56" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Biomass boiler_SH</v>
-      </c>
-      <c r="AU56" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV56" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV56" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY56" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -26360,19 +26355,19 @@
         <v/>
       </c>
       <c r="AK57" s="214">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL57" s="210"/>
       <c r="AM57" s="208">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN57" s="211"/>
       <c r="AO57" s="211"/>
       <c r="AP57" s="172"/>
       <c r="AQ57" s="45" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR57" s="45" t="str">
@@ -26380,25 +26375,25 @@
         <v>IE,National</v>
       </c>
       <c r="AS57" s="45" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS_BIO_N2</v>
+      </c>
+      <c r="AT57" s="45" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Biomass boiler_SH-WH</v>
+      </c>
+      <c r="AU57" s="45" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS_BIO_N2</v>
-      </c>
-      <c r="AT57" s="45" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Biomass boiler_SH-WH</v>
-      </c>
-      <c r="AU57" s="45" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV57" s="45" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV57" s="45" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AW57" s="45"/>
       <c r="AX57" s="45"/>
       <c r="AY57" s="45" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -26454,7 +26449,7 @@
       <c r="AO58" s="211"/>
       <c r="AP58" s="172"/>
       <c r="AQ58" s="57" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>*Heaters</v>
       </c>
       <c r="AR58" s="57" t="str">
@@ -26462,25 +26457,25 @@
         <v/>
       </c>
       <c r="AS58" s="57" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="AT58" s="57" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="AU58" s="57" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
-      <c r="AT58" s="57" t="str">
-        <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="AU58" s="57" t="str">
+      <c r="AV58" s="57" t="str">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="AV58" s="57" t="str">
-        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="AW58" s="57"/>
       <c r="AX58" s="57"/>
       <c r="AY58" s="57" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -26617,14 +26612,14 @@
       </c>
       <c r="AL59" s="46"/>
       <c r="AM59" s="82">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN59" s="211"/>
       <c r="AO59" s="211"/>
       <c r="AP59" s="172"/>
       <c r="AQ59" s="45" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR59" s="45" t="str">
@@ -26632,25 +26627,25 @@
         <v>IE,National</v>
       </c>
       <c r="AS59" s="45" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS_ELC_N1</v>
+      </c>
+      <c r="AT59" s="45" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Electric boiler_SH</v>
+      </c>
+      <c r="AU59" s="45" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS_ELC_N1</v>
-      </c>
-      <c r="AT59" s="45" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Electric boiler_SH</v>
-      </c>
-      <c r="AU59" s="45" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV59" s="45" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV59" s="45" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AW59" s="45"/>
       <c r="AX59" s="45"/>
       <c r="AY59" s="45" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -26706,7 +26701,7 @@
       <c r="AO60" s="211"/>
       <c r="AP60" s="172"/>
       <c r="AQ60" s="57" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>*Heat Pumps</v>
       </c>
       <c r="AR60" s="57" t="str">
@@ -26714,25 +26709,25 @@
         <v/>
       </c>
       <c r="AS60" s="57" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="AT60" s="57" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="AU60" s="57" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
-      <c r="AT60" s="57" t="str">
-        <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="AU60" s="57" t="str">
+      <c r="AV60" s="57" t="str">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="AV60" s="57" t="str">
-        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="AW60" s="57"/>
       <c r="AX60" s="57"/>
       <c r="AY60" s="57" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -26867,19 +26862,19 @@
         <v/>
       </c>
       <c r="AK61" s="68">
-        <f t="shared" ref="AK61:AK70" si="32">IF($A61="*","",31.536)</f>
+        <f t="shared" ref="AK61:AK70" si="31">IF($A61="*","",31.536)</f>
         <v>31.536000000000001</v>
       </c>
       <c r="AL61" s="40"/>
       <c r="AM61" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN61" s="211"/>
       <c r="AO61" s="211"/>
       <c r="AP61" s="172"/>
       <c r="AQ61" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR61" s="42" t="str">
@@ -26887,23 +26882,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS61" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS_ELC_N2</v>
+      </c>
+      <c r="AT61" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Heat Pump Air-to-Air_SH</v>
+      </c>
+      <c r="AU61" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS_ELC_N2</v>
-      </c>
-      <c r="AT61" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Heat Pump Air-to-Air_SH</v>
-      </c>
-      <c r="AU61" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV61" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV61" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY61" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -27038,19 +27033,19 @@
         <v/>
       </c>
       <c r="AK62" s="68">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL62" s="40"/>
       <c r="AM62" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN62" s="211"/>
       <c r="AO62" s="211"/>
       <c r="AP62" s="172"/>
       <c r="AQ62" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR62" s="42" t="str">
@@ -27058,23 +27053,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS62" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS_ELC_N3</v>
+      </c>
+      <c r="AT62" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Heat Pump Air-to-Air_SH-SC</v>
+      </c>
+      <c r="AU62" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS_ELC_N3</v>
-      </c>
-      <c r="AT62" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Heat Pump Air-to-Air_SH-SC</v>
-      </c>
-      <c r="AU62" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV62" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV62" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY62" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -27209,19 +27204,19 @@
         <v/>
       </c>
       <c r="AK63" s="68">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL63" s="40"/>
       <c r="AM63" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN63" s="211"/>
       <c r="AO63" s="211"/>
       <c r="AP63" s="172"/>
       <c r="AQ63" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR63" s="42" t="str">
@@ -27229,23 +27224,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS63" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS_ELC_N4</v>
+      </c>
+      <c r="AT63" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Heat Pump Air-to-Water_SH</v>
+      </c>
+      <c r="AU63" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS_ELC_N4</v>
-      </c>
-      <c r="AT63" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Heat Pump Air-to-Water_SH</v>
-      </c>
-      <c r="AU63" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV63" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV63" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY63" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -27380,19 +27375,19 @@
         <v/>
       </c>
       <c r="AK64" s="68">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL64" s="40"/>
       <c r="AM64" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN64" s="211"/>
       <c r="AO64" s="211"/>
       <c r="AP64" s="172"/>
       <c r="AQ64" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR64" s="42" t="str">
@@ -27400,23 +27395,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS64" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS_ELC_N5</v>
+      </c>
+      <c r="AT64" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Heat Pump Air-to-Water_SH-WH</v>
+      </c>
+      <c r="AU64" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS_ELC_N5</v>
-      </c>
-      <c r="AT64" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Heat Pump Air-to-Water_SH-WH</v>
-      </c>
-      <c r="AU64" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV64" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV64" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY64" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -27551,19 +27546,19 @@
         <v/>
       </c>
       <c r="AK65" s="68">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL65" s="40"/>
       <c r="AM65" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN65" s="211"/>
       <c r="AO65" s="211"/>
       <c r="AP65" s="172"/>
       <c r="AQ65" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR65" s="42" t="str">
@@ -27571,23 +27566,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS65" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS_ELC_N6</v>
+      </c>
+      <c r="AT65" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Heat Pump Air-to-Water + Solar thermal_SH-WH</v>
+      </c>
+      <c r="AU65" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS_ELC_N6</v>
-      </c>
-      <c r="AT65" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Heat Pump Air-to-Water + Solar thermal_SH-WH</v>
-      </c>
-      <c r="AU65" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV65" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV65" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY65" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -27722,19 +27717,19 @@
         <v/>
       </c>
       <c r="AK66" s="68">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL66" s="40"/>
       <c r="AM66" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN66" s="211"/>
       <c r="AO66" s="211"/>
       <c r="AP66" s="172"/>
       <c r="AQ66" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR66" s="42" t="str">
@@ -27742,23 +27737,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS66" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS_ELC_N7</v>
+      </c>
+      <c r="AT66" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Heat Pump Ground Source_SH</v>
+      </c>
+      <c r="AU66" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS_ELC_N7</v>
-      </c>
-      <c r="AT66" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Heat Pump Ground Source_SH</v>
-      </c>
-      <c r="AU66" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV66" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV66" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY66" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -27893,19 +27888,19 @@
         <v/>
       </c>
       <c r="AK67" s="68">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL67" s="40"/>
       <c r="AM67" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN67" s="211"/>
       <c r="AO67" s="211"/>
       <c r="AP67" s="172"/>
       <c r="AQ67" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR67" s="42" t="str">
@@ -27913,23 +27908,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS67" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS_ELC_N8</v>
+      </c>
+      <c r="AT67" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Heat Pump Ground Source_SH-SC</v>
+      </c>
+      <c r="AU67" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS_ELC_N8</v>
-      </c>
-      <c r="AT67" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Heat Pump Ground Source_SH-SC</v>
-      </c>
-      <c r="AU67" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV67" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV67" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY67" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -28064,19 +28059,19 @@
         <v/>
       </c>
       <c r="AK68" s="68">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL68" s="40"/>
       <c r="AM68" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN68" s="211"/>
       <c r="AO68" s="211"/>
       <c r="AP68" s="172"/>
       <c r="AQ68" s="42" t="str">
-        <f t="shared" ref="AQ68" si="33">IF(LEFT(A68)="*",A68,"PRE")</f>
+        <f t="shared" ref="AQ68" si="32">IF(LEFT(A68)="*",A68,"PRE")</f>
         <v>PRE</v>
       </c>
       <c r="AR68" s="42" t="str">
@@ -28084,23 +28079,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS68" s="42" t="str">
-        <f t="shared" ref="AS68" si="34">IF(LEFT($A68)="*","",A68)</f>
+        <f t="shared" ref="AS68" si="33">IF(LEFT($A68)="*","",A68)</f>
         <v>S-SH-CS_ELC_N9</v>
       </c>
       <c r="AT68" s="42" t="str">
-        <f t="shared" ref="AT68" si="35">IF(LEFT($A68)="*","",B68)</f>
+        <f t="shared" ref="AT68" si="34">IF(LEFT($A68)="*","",B68)</f>
         <v>Commercial Services - Centralized Air-to-Air heat pump_SH-SC</v>
       </c>
       <c r="AU68" s="42" t="str">
+        <f t="shared" si="25"/>
+        <v>PJ</v>
+      </c>
+      <c r="AV68" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV68" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY68" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -28235,19 +28230,19 @@
         <v/>
       </c>
       <c r="AK69" s="68">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL69" s="40"/>
       <c r="AM69" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN69" s="211"/>
       <c r="AO69" s="211"/>
       <c r="AP69" s="172"/>
       <c r="AQ69" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR69" s="42" t="str">
@@ -28255,23 +28250,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS69" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS_GAS_N5</v>
+      </c>
+      <c r="AT69" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Gas-driven Heat Pump absorption_SH-WH</v>
+      </c>
+      <c r="AU69" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS_GAS_N5</v>
-      </c>
-      <c r="AT69" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Gas-driven Heat Pump absorption_SH-WH</v>
-      </c>
-      <c r="AU69" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV69" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV69" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY69" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -28406,19 +28401,19 @@
         <v/>
       </c>
       <c r="AK70" s="69">
-        <f t="shared" si="32"/>
+        <f t="shared" si="31"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL70" s="46"/>
       <c r="AM70" s="82">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN70" s="172"/>
       <c r="AO70" s="172"/>
       <c r="AP70" s="172"/>
       <c r="AQ70" s="45" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR70" s="45" t="str">
@@ -28426,25 +28421,25 @@
         <v>IE,National</v>
       </c>
       <c r="AS70" s="45" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS_GAS_N6</v>
+      </c>
+      <c r="AT70" s="45" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Gas-driven Heat Pump engine_SH-WH</v>
+      </c>
+      <c r="AU70" s="45" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS_GAS_N6</v>
-      </c>
-      <c r="AT70" s="45" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Gas-driven Heat Pump engine_SH-WH</v>
-      </c>
-      <c r="AU70" s="45" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV70" s="45" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV70" s="45" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AW70" s="45"/>
       <c r="AX70" s="45"/>
       <c r="AY70" s="45" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -28500,7 +28495,7 @@
       <c r="AO71" s="172"/>
       <c r="AP71" s="172"/>
       <c r="AQ71" s="57" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>*District Heating</v>
       </c>
       <c r="AR71" s="57" t="str">
@@ -28508,25 +28503,25 @@
         <v/>
       </c>
       <c r="AS71" s="57" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="AT71" s="57" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="AU71" s="57" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
-      <c r="AT71" s="57" t="str">
-        <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="AU71" s="57" t="str">
+      <c r="AV71" s="57" t="str">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="AV71" s="57" t="str">
-        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="AW71" s="57"/>
       <c r="AX71" s="57"/>
       <c r="AY71" s="57" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -28589,23 +28584,23 @@
       </c>
       <c r="P72" s="262">
         <f>IF($A72="*","",IF(SRV_TH!P29=0,"",SRV_TH!P29))</f>
-        <v>1.4</v>
+        <v>1.29</v>
       </c>
       <c r="Q72" s="262">
         <f>IF($A72="*","",IF(SRV_TH!Q29=0,"",SRV_TH!Q29))</f>
-        <v>1.4</v>
+        <v>1.29</v>
       </c>
       <c r="R72" s="262">
         <f>IF($A72="*","",IF(SRV_TH!R29=0,"",SRV_TH!R29))</f>
-        <v>1.4</v>
+        <v>1.29</v>
       </c>
       <c r="S72" s="262">
         <f>IF($A72="*","",IF(SRV_TH!S29=0,"",SRV_TH!S29))</f>
-        <v>1.4</v>
+        <v>1.29</v>
       </c>
       <c r="T72" s="262">
         <f>IF($A72="*","",IF(SRV_TH!T29=0,"",SRV_TH!T29))</f>
-        <v>1.4</v>
+        <v>1.29</v>
       </c>
       <c r="U72" s="212">
         <f>IF($A72="*","",IF(SRV_TH!U29=0,"",SRV_TH!U29))</f>
@@ -28662,14 +28657,14 @@
       </c>
       <c r="AL72" s="210"/>
       <c r="AM72" s="208">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN72" s="176"/>
       <c r="AO72" s="176"/>
       <c r="AP72" s="172"/>
       <c r="AQ72" s="45" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR72" s="45" t="str">
@@ -28677,25 +28672,25 @@
         <v>IE,National</v>
       </c>
       <c r="AS72" s="45" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SH-CS_HET_N1</v>
+      </c>
+      <c r="AT72" s="45" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Centralized DistrictH_Heat Exchanger_SH-WH</v>
+      </c>
+      <c r="AU72" s="45" t="str">
         <f t="shared" si="25"/>
-        <v>S-SH-CS_HET_N1</v>
-      </c>
-      <c r="AT72" s="45" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Centralized DistrictH_Heat Exchanger_SH-WH</v>
-      </c>
-      <c r="AU72" s="45" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV72" s="45" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV72" s="45" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AW72" s="45"/>
       <c r="AX72" s="45"/>
       <c r="AY72" s="45" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -28751,7 +28746,7 @@
       <c r="AO73" s="172"/>
       <c r="AP73" s="172"/>
       <c r="AQ73" s="57" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>*Water Heat-only</v>
       </c>
       <c r="AR73" s="57" t="str">
@@ -28759,25 +28754,25 @@
         <v/>
       </c>
       <c r="AS73" s="57" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="AT73" s="57" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="AU73" s="57" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
-      <c r="AT73" s="57" t="str">
-        <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="AU73" s="57" t="str">
+      <c r="AV73" s="57" t="str">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="AV73" s="57" t="str">
-        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="AW73" s="57"/>
       <c r="AX73" s="57"/>
       <c r="AY73" s="57" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -28913,14 +28908,14 @@
       </c>
       <c r="AL74" s="84"/>
       <c r="AM74" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN74" s="172"/>
       <c r="AO74" s="172"/>
       <c r="AP74" s="172"/>
       <c r="AQ74" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR74" s="42" t="str">
@@ -28928,23 +28923,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS74" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-WH-CS_ELC_N1</v>
+      </c>
+      <c r="AT74" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Electric water heater_WH</v>
+      </c>
+      <c r="AU74" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-WH-CS_ELC_N1</v>
-      </c>
-      <c r="AT74" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Electric water heater_WH</v>
-      </c>
-      <c r="AU74" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV74" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV74" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY74" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -29080,14 +29075,14 @@
       </c>
       <c r="AL75" s="40"/>
       <c r="AM75" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN75" s="172"/>
       <c r="AO75" s="172"/>
       <c r="AP75" s="172"/>
       <c r="AQ75" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR75" s="42" t="str">
@@ -29095,23 +29090,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS75" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-WH-CS_SOL_N1</v>
+      </c>
+      <c r="AT75" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Solar water heater_WH</v>
+      </c>
+      <c r="AU75" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-WH-CS_SOL_N1</v>
-      </c>
-      <c r="AT75" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Solar water heater_WH</v>
-      </c>
-      <c r="AU75" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV75" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV75" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY75" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -29247,14 +29242,14 @@
       </c>
       <c r="AL76" s="84"/>
       <c r="AM76" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN76" s="172"/>
       <c r="AO76" s="172"/>
       <c r="AP76" s="172"/>
       <c r="AQ76" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR76" s="42" t="str">
@@ -29262,23 +29257,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS76" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-WH-CS_GAS_N1</v>
+      </c>
+      <c r="AT76" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Gas water heater_WH</v>
+      </c>
+      <c r="AU76" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-WH-CS_GAS_N1</v>
-      </c>
-      <c r="AT76" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Gas water heater_WH</v>
-      </c>
-      <c r="AU76" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV76" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV76" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY76" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -29409,19 +29404,19 @@
         <v/>
       </c>
       <c r="AK77" s="68">
-        <f t="shared" ref="AK77:AK78" si="36">IF($A77="*","",31.536)</f>
+        <f t="shared" ref="AK77:AK78" si="35">IF($A77="*","",31.536)</f>
         <v>31.536000000000001</v>
       </c>
       <c r="AL77" s="84"/>
       <c r="AM77" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN77" s="172"/>
       <c r="AO77" s="172"/>
       <c r="AP77" s="172"/>
       <c r="AQ77" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR77" s="42" t="str">
@@ -29429,23 +29424,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS77" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-WH-CS_BIO_N1</v>
+      </c>
+      <c r="AT77" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Biomass water heater_WH</v>
+      </c>
+      <c r="AU77" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-WH-CS_BIO_N1</v>
-      </c>
-      <c r="AT77" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Biomass water heater_WH</v>
-      </c>
-      <c r="AU77" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV77" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV77" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY77" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -29577,19 +29572,19 @@
         <v/>
       </c>
       <c r="AK78" s="214">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL78" s="71"/>
       <c r="AM78" s="208">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN78" s="211"/>
       <c r="AO78" s="211"/>
       <c r="AP78" s="172"/>
       <c r="AQ78" s="45" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR78" s="45" t="str">
@@ -29597,25 +29592,25 @@
         <v>IE,National</v>
       </c>
       <c r="AS78" s="45" t="str">
+        <f t="shared" si="24"/>
+        <v>S-WH-CS_LPG_N1</v>
+      </c>
+      <c r="AT78" s="45" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - LPG water heater_WH</v>
+      </c>
+      <c r="AU78" s="45" t="str">
         <f t="shared" si="25"/>
-        <v>S-WH-CS_LPG_N1</v>
-      </c>
-      <c r="AT78" s="45" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - LPG water heater_WH</v>
-      </c>
-      <c r="AU78" s="45" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV78" s="45" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV78" s="45" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AW78" s="45"/>
       <c r="AX78" s="45"/>
       <c r="AY78" s="45" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -29671,7 +29666,7 @@
       <c r="AO79" s="211"/>
       <c r="AP79" s="172"/>
       <c r="AQ79" s="57" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>*Cooling-only</v>
       </c>
       <c r="AR79" s="57" t="str">
@@ -29679,25 +29674,25 @@
         <v/>
       </c>
       <c r="AS79" s="57" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="AT79" s="57" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+      <c r="AU79" s="57" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
-      <c r="AT79" s="57" t="str">
-        <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="AU79" s="57" t="str">
+      <c r="AV79" s="57" t="str">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="AV79" s="57" t="str">
-        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="AW79" s="57"/>
       <c r="AX79" s="57"/>
       <c r="AY79" s="57" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -29833,14 +29828,14 @@
       </c>
       <c r="AL80" s="84"/>
       <c r="AM80" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AN80" s="172"/>
       <c r="AO80" s="172"/>
       <c r="AP80" s="172"/>
       <c r="AQ80" s="42" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>PRE</v>
       </c>
       <c r="AR80" s="42" t="str">
@@ -29848,23 +29843,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS80" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>S-SC-CS_ELC_N1</v>
+      </c>
+      <c r="AT80" s="42" t="str">
+        <f t="shared" si="24"/>
+        <v>Commercial Services - Room air conditioning Air-to-Air_SC</v>
+      </c>
+      <c r="AU80" s="42" t="str">
         <f t="shared" si="25"/>
-        <v>S-SC-CS_ELC_N1</v>
-      </c>
-      <c r="AT80" s="42" t="str">
-        <f t="shared" si="25"/>
-        <v>Commercial Services - Room air conditioning Air-to-Air_SC</v>
-      </c>
-      <c r="AU80" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV80" s="42" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV80" s="42" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AY80" s="42" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -30001,11 +29996,11 @@
       </c>
       <c r="AL81" s="71"/>
       <c r="AM81" s="208">
-        <f t="shared" si="30"/>
+        <f t="shared" si="29"/>
         <v>2019</v>
       </c>
       <c r="AQ81" s="45" t="str">
-        <f t="shared" ref="AQ81" si="37">IF(LEFT(A81)="*",A81,"PRE")</f>
+        <f t="shared" ref="AQ81" si="36">IF(LEFT(A81)="*",A81,"PRE")</f>
         <v>PRE</v>
       </c>
       <c r="AR81" s="45" t="str">
@@ -30013,25 +30008,25 @@
         <v>IE,National</v>
       </c>
       <c r="AS81" s="45" t="str">
-        <f t="shared" ref="AS81" si="38">IF(LEFT($A81)="*","",A81)</f>
+        <f t="shared" ref="AS81" si="37">IF(LEFT($A81)="*","",A81)</f>
         <v>S-SC-CS_ELC_N2</v>
       </c>
       <c r="AT81" s="45" t="str">
-        <f t="shared" ref="AT81" si="39">IF(LEFT($A81)="*","",B81)</f>
+        <f t="shared" ref="AT81" si="38">IF(LEFT($A81)="*","",B81)</f>
         <v>Commercial Services - Centralized air conditioning_SC</v>
       </c>
       <c r="AU81" s="45" t="str">
+        <f t="shared" si="25"/>
+        <v>PJ</v>
+      </c>
+      <c r="AV81" s="45" t="str">
         <f t="shared" si="26"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV81" s="45" t="str">
-        <f t="shared" si="27"/>
         <v>GW</v>
       </c>
       <c r="AW81" s="45"/>
       <c r="AX81" s="45"/>
       <c r="AY81" s="45" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="30"/>
         <v>YES</v>
       </c>
     </row>
@@ -30555,7 +30550,7 @@
       <c r="AO88" s="211"/>
       <c r="AP88" s="172"/>
       <c r="AQ88" s="224" t="str">
-        <f t="shared" ref="AQ88:AQ121" si="40">IF(LEFT(A88)="*",A88,"PRE")</f>
+        <f t="shared" ref="AQ88:AQ121" si="39">IF(LEFT(A88)="*",A88,"PRE")</f>
         <v>*Boilers</v>
       </c>
       <c r="AR88" s="224" t="str">
@@ -30563,19 +30558,19 @@
         <v/>
       </c>
       <c r="AS88" s="224" t="str">
-        <f t="shared" ref="AS88:AT121" si="41">IF(LEFT($A88)="*","",A88)</f>
+        <f t="shared" ref="AS88:AT121" si="40">IF(LEFT($A88)="*","",A88)</f>
         <v/>
       </c>
       <c r="AT88" s="224" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="AU88" s="224" t="str">
-        <f t="shared" ref="AU88:AU122" si="42">IF(LEFT($A88)="*","","PJ")</f>
+        <f t="shared" ref="AU88:AU122" si="41">IF(LEFT($A88)="*","","PJ")</f>
         <v/>
       </c>
       <c r="AV88" s="224" t="str">
-        <f t="shared" ref="AV88:AV122" si="43">IF(LEFT($A88)="*","","GW")</f>
+        <f t="shared" ref="AV88:AV122" si="42">IF(LEFT($A88)="*","","GW")</f>
         <v/>
       </c>
       <c r="AW88" s="42" t="str">
@@ -30584,7 +30579,7 @@
       </c>
       <c r="AX88" s="224"/>
       <c r="AY88" s="224" t="str">
-        <f t="shared" ref="AY88:AY122" si="44">IF($AS88="","","YES")</f>
+        <f t="shared" ref="AY88:AY122" si="43">IF($AS88="","","YES")</f>
         <v/>
       </c>
     </row>
@@ -30715,7 +30710,7 @@
         <v/>
       </c>
       <c r="AK89" s="68">
-        <f t="shared" ref="AK89:AK98" si="45">IF($A89="*","",31.536)</f>
+        <f t="shared" ref="AK89:AK98" si="44">IF($A89="*","",31.536)</f>
         <v>31.536000000000001</v>
       </c>
       <c r="AL89" s="40"/>
@@ -30727,7 +30722,7 @@
       <c r="AO89" s="211"/>
       <c r="AP89" s="172"/>
       <c r="AQ89" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR89" s="42" t="str">
@@ -30735,23 +30730,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS89" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_OIL_N1</v>
+      </c>
+      <c r="AT89" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Oil boiler condensing_SH</v>
+      </c>
+      <c r="AU89" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_OIL_N1</v>
-      </c>
-      <c r="AT89" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Oil boiler condensing_SH</v>
-      </c>
-      <c r="AU89" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV89" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV89" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY89" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY89" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -30882,19 +30877,19 @@
         <v/>
       </c>
       <c r="AK90" s="68">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL90" s="40"/>
       <c r="AM90" s="81">
-        <f t="shared" ref="AM90:AM122" si="46">IF($A90="*","",2019)</f>
+        <f t="shared" ref="AM90:AM122" si="45">IF($A90="*","",2019)</f>
         <v>2019</v>
       </c>
       <c r="AN90" s="211"/>
       <c r="AO90" s="211"/>
       <c r="AP90" s="172"/>
       <c r="AQ90" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR90" s="42" t="str">
@@ -30902,23 +30897,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS90" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_OIL_N2</v>
+      </c>
+      <c r="AT90" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Oil boiler condensing_SH-WH</v>
+      </c>
+      <c r="AU90" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_OIL_N2</v>
-      </c>
-      <c r="AT90" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Oil boiler condensing_SH-WH</v>
-      </c>
-      <c r="AU90" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV90" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV90" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY90" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY90" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -31049,19 +31044,19 @@
         <v/>
       </c>
       <c r="AK91" s="68">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL91" s="40"/>
       <c r="AM91" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN91" s="211"/>
       <c r="AO91" s="211"/>
       <c r="AP91" s="172"/>
       <c r="AQ91" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR91" s="42" t="str">
@@ -31069,23 +31064,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS91" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_GAS_N1</v>
+      </c>
+      <c r="AT91" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Gas boiler condensing_SH</v>
+      </c>
+      <c r="AU91" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_GAS_N1</v>
-      </c>
-      <c r="AT91" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Gas boiler condensing_SH</v>
-      </c>
-      <c r="AU91" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV91" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV91" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY91" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY91" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -31216,19 +31211,19 @@
         <v/>
       </c>
       <c r="AK92" s="68">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL92" s="40"/>
       <c r="AM92" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN92" s="211"/>
       <c r="AO92" s="211"/>
       <c r="AP92" s="172"/>
       <c r="AQ92" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR92" s="42" t="str">
@@ -31236,23 +31231,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS92" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_GAS_N2</v>
+      </c>
+      <c r="AT92" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve">Public Services - Gas boiler condensing_SH-WH </v>
+      </c>
+      <c r="AU92" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_GAS_N2</v>
-      </c>
-      <c r="AT92" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v xml:space="preserve">Public Services - Gas boiler condensing_SH-WH </v>
-      </c>
-      <c r="AU92" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV92" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV92" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY92" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY92" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -31383,19 +31378,19 @@
         <v/>
       </c>
       <c r="AK93" s="68">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL93" s="40"/>
       <c r="AM93" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN93" s="211"/>
       <c r="AO93" s="211"/>
       <c r="AP93" s="172"/>
       <c r="AQ93" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR93" s="42" t="str">
@@ -31403,23 +31398,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS93" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_GAS_N3</v>
+      </c>
+      <c r="AT93" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve">Public Services - Gas boiler condensing + Solar thermal_SH-WH </v>
+      </c>
+      <c r="AU93" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_GAS_N3</v>
-      </c>
-      <c r="AT93" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v xml:space="preserve">Public Services - Gas boiler condensing + Solar thermal_SH-WH </v>
-      </c>
-      <c r="AU93" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV93" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV93" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY93" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY93" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -31550,19 +31545,19 @@
         <v>0.51127819548872178</v>
       </c>
       <c r="AK94" s="68">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL94" s="40"/>
       <c r="AM94" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN94" s="211"/>
       <c r="AO94" s="211"/>
       <c r="AP94" s="172"/>
       <c r="AQ94" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR94" s="42" t="str">
@@ -31570,23 +31565,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS94" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_GAS_N4</v>
+      </c>
+      <c r="AT94" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve">Public Services - Gas boiler condensing + Wood stove_SH-WH </v>
+      </c>
+      <c r="AU94" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_GAS_N4</v>
-      </c>
-      <c r="AT94" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v xml:space="preserve">Public Services - Gas boiler condensing + Wood stove_SH-WH </v>
-      </c>
-      <c r="AU94" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV94" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV94" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY94" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY94" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -31717,19 +31712,19 @@
         <v/>
       </c>
       <c r="AK95" s="68">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL95" s="84"/>
       <c r="AM95" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN95" s="211"/>
       <c r="AO95" s="211"/>
       <c r="AP95" s="172"/>
       <c r="AQ95" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR95" s="42" t="str">
@@ -31737,23 +31732,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS95" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_LPG_N1</v>
+      </c>
+      <c r="AT95" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - LPG boiler condensing_SH</v>
+      </c>
+      <c r="AU95" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_LPG_N1</v>
-      </c>
-      <c r="AT95" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - LPG boiler condensing_SH</v>
-      </c>
-      <c r="AU95" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV95" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV95" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY95" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY95" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -31884,19 +31879,19 @@
         <v/>
       </c>
       <c r="AK96" s="68">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL96" s="84"/>
       <c r="AM96" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN96" s="211"/>
       <c r="AO96" s="211"/>
       <c r="AP96" s="172"/>
       <c r="AQ96" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR96" s="42" t="str">
@@ -31904,23 +31899,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS96" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_LPG_N2</v>
+      </c>
+      <c r="AT96" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - LPG boiler condensing_SH-WH</v>
+      </c>
+      <c r="AU96" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_LPG_N2</v>
-      </c>
-      <c r="AT96" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - LPG boiler condensing_SH-WH</v>
-      </c>
-      <c r="AU96" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV96" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV96" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY96" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY96" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -32052,19 +32047,19 @@
         <v/>
       </c>
       <c r="AK97" s="68">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL97" s="40"/>
       <c r="AM97" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN97" s="211"/>
       <c r="AO97" s="211"/>
       <c r="AP97" s="172"/>
       <c r="AQ97" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR97" s="42" t="str">
@@ -32072,23 +32067,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS97" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_BIO_N1</v>
+      </c>
+      <c r="AT97" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Biomass boiler_SH</v>
+      </c>
+      <c r="AU97" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_BIO_N1</v>
-      </c>
-      <c r="AT97" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Biomass boiler_SH</v>
-      </c>
-      <c r="AU97" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV97" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV97" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY97" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY97" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -32220,19 +32215,19 @@
         <v/>
       </c>
       <c r="AK98" s="214">
-        <f t="shared" si="45"/>
+        <f t="shared" si="44"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL98" s="210"/>
       <c r="AM98" s="208">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN98" s="211"/>
       <c r="AO98" s="211"/>
       <c r="AP98" s="172"/>
       <c r="AQ98" s="45" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR98" s="45" t="str">
@@ -32240,25 +32235,25 @@
         <v>IE,National</v>
       </c>
       <c r="AS98" s="45" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_BIO_N2</v>
+      </c>
+      <c r="AT98" s="45" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Biomass boiler_SH-WH</v>
+      </c>
+      <c r="AU98" s="45" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_BIO_N2</v>
-      </c>
-      <c r="AT98" s="45" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Biomass boiler_SH-WH</v>
-      </c>
-      <c r="AU98" s="45" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV98" s="45" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV98" s="45" t="str">
-        <f t="shared" si="43"/>
         <v>GW</v>
       </c>
       <c r="AW98" s="45"/>
       <c r="AX98" s="45"/>
       <c r="AY98" s="45" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>YES</v>
       </c>
     </row>
@@ -32314,7 +32309,7 @@
       <c r="AO99" s="211"/>
       <c r="AP99" s="172"/>
       <c r="AQ99" s="57" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>*Heaters</v>
       </c>
       <c r="AR99" s="57" t="str">
@@ -32322,25 +32317,25 @@
         <v/>
       </c>
       <c r="AS99" s="57" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="AT99" s="57" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="AU99" s="57" t="str">
         <f t="shared" si="41"/>
         <v/>
       </c>
-      <c r="AT99" s="57" t="str">
-        <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="AU99" s="57" t="str">
+      <c r="AV99" s="57" t="str">
         <f t="shared" si="42"/>
-        <v/>
-      </c>
-      <c r="AV99" s="57" t="str">
-        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AW99" s="57"/>
       <c r="AX99" s="57"/>
       <c r="AY99" s="57" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
@@ -32477,14 +32472,14 @@
       </c>
       <c r="AL100" s="46"/>
       <c r="AM100" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN100" s="211"/>
       <c r="AO100" s="211"/>
       <c r="AP100" s="172"/>
       <c r="AQ100" s="45" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR100" s="45" t="str">
@@ -32492,25 +32487,25 @@
         <v>IE,National</v>
       </c>
       <c r="AS100" s="45" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_ELC_N1</v>
+      </c>
+      <c r="AT100" s="45" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Electric boiler_SH</v>
+      </c>
+      <c r="AU100" s="45" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_ELC_N1</v>
-      </c>
-      <c r="AT100" s="45" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Electric boiler_SH</v>
-      </c>
-      <c r="AU100" s="45" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV100" s="45" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV100" s="45" t="str">
-        <f t="shared" si="43"/>
         <v>GW</v>
       </c>
       <c r="AW100" s="45"/>
       <c r="AX100" s="45"/>
       <c r="AY100" s="45" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>YES</v>
       </c>
     </row>
@@ -32566,7 +32561,7 @@
       <c r="AO101" s="211"/>
       <c r="AP101" s="172"/>
       <c r="AQ101" s="57" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>*Heat Pumps</v>
       </c>
       <c r="AR101" s="57" t="str">
@@ -32574,25 +32569,25 @@
         <v/>
       </c>
       <c r="AS101" s="57" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="AT101" s="57" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="AU101" s="57" t="str">
         <f t="shared" si="41"/>
         <v/>
       </c>
-      <c r="AT101" s="57" t="str">
-        <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="AU101" s="57" t="str">
+      <c r="AV101" s="57" t="str">
         <f t="shared" si="42"/>
-        <v/>
-      </c>
-      <c r="AV101" s="57" t="str">
-        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AW101" s="57"/>
       <c r="AX101" s="57"/>
       <c r="AY101" s="57" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
@@ -32727,19 +32722,19 @@
         <v/>
       </c>
       <c r="AK102" s="68">
-        <f t="shared" ref="AK102:AK111" si="47">IF($A102="*","",31.536)</f>
+        <f t="shared" ref="AK102:AK111" si="46">IF($A102="*","",31.536)</f>
         <v>31.536000000000001</v>
       </c>
       <c r="AL102" s="40"/>
       <c r="AM102" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN102" s="211"/>
       <c r="AO102" s="211"/>
       <c r="AP102" s="172"/>
       <c r="AQ102" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR102" s="42" t="str">
@@ -32747,23 +32742,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS102" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_ELC_N2</v>
+      </c>
+      <c r="AT102" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Heat Pump Air-to-Air_SH</v>
+      </c>
+      <c r="AU102" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_ELC_N2</v>
-      </c>
-      <c r="AT102" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Heat Pump Air-to-Air_SH</v>
-      </c>
-      <c r="AU102" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV102" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV102" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY102" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY102" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -32898,19 +32893,19 @@
         <v/>
       </c>
       <c r="AK103" s="68">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL103" s="40"/>
       <c r="AM103" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN103" s="211"/>
       <c r="AO103" s="211"/>
       <c r="AP103" s="172"/>
       <c r="AQ103" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR103" s="42" t="str">
@@ -32918,23 +32913,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS103" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_ELC_N3</v>
+      </c>
+      <c r="AT103" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Heat Pump Air-to-Air_SH-SC</v>
+      </c>
+      <c r="AU103" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_ELC_N3</v>
-      </c>
-      <c r="AT103" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Heat Pump Air-to-Air_SH-SC</v>
-      </c>
-      <c r="AU103" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV103" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV103" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY103" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY103" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -33069,19 +33064,19 @@
         <v/>
       </c>
       <c r="AK104" s="68">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL104" s="40"/>
       <c r="AM104" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN104" s="211"/>
       <c r="AO104" s="211"/>
       <c r="AP104" s="172"/>
       <c r="AQ104" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR104" s="42" t="str">
@@ -33089,23 +33084,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS104" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_ELC_N4</v>
+      </c>
+      <c r="AT104" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Heat Pump Air-to-Water_SH</v>
+      </c>
+      <c r="AU104" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_ELC_N4</v>
-      </c>
-      <c r="AT104" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Heat Pump Air-to-Water_SH</v>
-      </c>
-      <c r="AU104" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV104" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV104" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY104" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY104" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -33240,19 +33235,19 @@
         <v/>
       </c>
       <c r="AK105" s="68">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL105" s="40"/>
       <c r="AM105" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN105" s="211"/>
       <c r="AO105" s="211"/>
       <c r="AP105" s="172"/>
       <c r="AQ105" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR105" s="42" t="str">
@@ -33260,23 +33255,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS105" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_ELC_N5</v>
+      </c>
+      <c r="AT105" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Heat Pump Air-to-Water_SH-WH</v>
+      </c>
+      <c r="AU105" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_ELC_N5</v>
-      </c>
-      <c r="AT105" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Heat Pump Air-to-Water_SH-WH</v>
-      </c>
-      <c r="AU105" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV105" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV105" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY105" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY105" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -33411,19 +33406,19 @@
         <v/>
       </c>
       <c r="AK106" s="68">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL106" s="40"/>
       <c r="AM106" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN106" s="211"/>
       <c r="AO106" s="211"/>
       <c r="AP106" s="172"/>
       <c r="AQ106" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR106" s="42" t="str">
@@ -33431,23 +33426,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS106" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_ELC_N6</v>
+      </c>
+      <c r="AT106" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Heat Pump Air-to-Water + Solar thermal_SH-WH</v>
+      </c>
+      <c r="AU106" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_ELC_N6</v>
-      </c>
-      <c r="AT106" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Heat Pump Air-to-Water + Solar thermal_SH-WH</v>
-      </c>
-      <c r="AU106" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV106" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV106" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY106" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY106" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -33582,19 +33577,19 @@
         <v/>
       </c>
       <c r="AK107" s="68">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL107" s="40"/>
       <c r="AM107" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN107" s="211"/>
       <c r="AO107" s="211"/>
       <c r="AP107" s="172"/>
       <c r="AQ107" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR107" s="42" t="str">
@@ -33602,23 +33597,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS107" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_ELC_N7</v>
+      </c>
+      <c r="AT107" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Heat Pump Ground Source_SH</v>
+      </c>
+      <c r="AU107" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_ELC_N7</v>
-      </c>
-      <c r="AT107" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Heat Pump Ground Source_SH</v>
-      </c>
-      <c r="AU107" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV107" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV107" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY107" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY107" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -33753,19 +33748,19 @@
         <v/>
       </c>
       <c r="AK108" s="68">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL108" s="40"/>
       <c r="AM108" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN108" s="211"/>
       <c r="AO108" s="211"/>
       <c r="AP108" s="172"/>
       <c r="AQ108" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR108" s="42" t="str">
@@ -33773,23 +33768,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS108" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_ELC_N8</v>
+      </c>
+      <c r="AT108" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Heat Pump Ground Source_SH-SC</v>
+      </c>
+      <c r="AU108" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_ELC_N8</v>
-      </c>
-      <c r="AT108" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Heat Pump Ground Source_SH-SC</v>
-      </c>
-      <c r="AU108" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV108" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV108" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY108" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY108" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -33924,19 +33919,19 @@
         <v/>
       </c>
       <c r="AK109" s="68">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL109" s="40"/>
       <c r="AM109" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN109" s="211"/>
       <c r="AO109" s="211"/>
       <c r="AP109" s="172"/>
       <c r="AQ109" s="42" t="str">
-        <f t="shared" ref="AQ109" si="48">IF(LEFT(A109)="*",A109,"PRE")</f>
+        <f t="shared" ref="AQ109" si="47">IF(LEFT(A109)="*",A109,"PRE")</f>
         <v>PRE</v>
       </c>
       <c r="AR109" s="42" t="str">
@@ -33944,23 +33939,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS109" s="42" t="str">
-        <f t="shared" ref="AS109" si="49">IF(LEFT($A109)="*","",A109)</f>
+        <f t="shared" ref="AS109" si="48">IF(LEFT($A109)="*","",A109)</f>
         <v>S-SH-PU_ELC_N9</v>
       </c>
       <c r="AT109" s="42" t="str">
-        <f t="shared" ref="AT109" si="50">IF(LEFT($A109)="*","",B109)</f>
+        <f t="shared" ref="AT109" si="49">IF(LEFT($A109)="*","",B109)</f>
         <v>Public Services - Centralized Air-to-Air heat pump_SH-SC</v>
       </c>
       <c r="AU109" s="42" t="str">
+        <f t="shared" si="41"/>
+        <v>PJ</v>
+      </c>
+      <c r="AV109" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV109" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY109" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY109" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -34095,19 +34090,19 @@
         <v/>
       </c>
       <c r="AK110" s="68">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL110" s="40"/>
       <c r="AM110" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN110" s="211"/>
       <c r="AO110" s="211"/>
       <c r="AP110" s="172"/>
       <c r="AQ110" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR110" s="42" t="str">
@@ -34115,23 +34110,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS110" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_GAS_N5</v>
+      </c>
+      <c r="AT110" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Gas-driven Heat Pump absorption_SH-WH</v>
+      </c>
+      <c r="AU110" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_GAS_N5</v>
-      </c>
-      <c r="AT110" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Gas-driven Heat Pump absorption_SH-WH</v>
-      </c>
-      <c r="AU110" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV110" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV110" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY110" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY110" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -34266,19 +34261,19 @@
         <v/>
       </c>
       <c r="AK111" s="69">
-        <f t="shared" si="47"/>
+        <f t="shared" si="46"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL111" s="46"/>
       <c r="AM111" s="82">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN111" s="211"/>
       <c r="AO111" s="211"/>
       <c r="AP111" s="172"/>
       <c r="AQ111" s="45" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR111" s="45" t="str">
@@ -34286,25 +34281,25 @@
         <v>IE,National</v>
       </c>
       <c r="AS111" s="45" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_GAS_N6</v>
+      </c>
+      <c r="AT111" s="45" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Gas-driven Heat Pump engine_SH-WH</v>
+      </c>
+      <c r="AU111" s="45" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_GAS_N6</v>
-      </c>
-      <c r="AT111" s="45" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Gas-driven Heat Pump engine_SH-WH</v>
-      </c>
-      <c r="AU111" s="45" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV111" s="45" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV111" s="45" t="str">
-        <f t="shared" si="43"/>
         <v>GW</v>
       </c>
       <c r="AW111" s="45"/>
       <c r="AX111" s="45"/>
       <c r="AY111" s="45" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>YES</v>
       </c>
     </row>
@@ -34360,7 +34355,7 @@
       <c r="AO112" s="211"/>
       <c r="AP112" s="172"/>
       <c r="AQ112" s="57" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>*District Heating</v>
       </c>
       <c r="AR112" s="57" t="str">
@@ -34368,25 +34363,25 @@
         <v/>
       </c>
       <c r="AS112" s="57" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="AT112" s="57" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="AU112" s="57" t="str">
         <f t="shared" si="41"/>
         <v/>
       </c>
-      <c r="AT112" s="57" t="str">
-        <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="AU112" s="57" t="str">
+      <c r="AV112" s="57" t="str">
         <f t="shared" si="42"/>
-        <v/>
-      </c>
-      <c r="AV112" s="57" t="str">
-        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AW112" s="57"/>
       <c r="AX112" s="57"/>
       <c r="AY112" s="57" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
@@ -34450,23 +34445,23 @@
       </c>
       <c r="P113" s="262">
         <f>IF($A113="*","",IF(SRV_TH!P29=0,"",SRV_TH!P29))</f>
-        <v>1.4</v>
+        <v>1.29</v>
       </c>
       <c r="Q113" s="262">
         <f>IF($A113="*","",IF(SRV_TH!Q29=0,"",SRV_TH!Q29))</f>
-        <v>1.4</v>
+        <v>1.29</v>
       </c>
       <c r="R113" s="262">
         <f>IF($A113="*","",IF(SRV_TH!R29=0,"",SRV_TH!R29))</f>
-        <v>1.4</v>
+        <v>1.29</v>
       </c>
       <c r="S113" s="262">
         <f>IF($A113="*","",IF(SRV_TH!S29=0,"",SRV_TH!S29))</f>
-        <v>1.4</v>
+        <v>1.29</v>
       </c>
       <c r="T113" s="262">
         <f>IF($A113="*","",IF(SRV_TH!T29=0,"",SRV_TH!T29))</f>
-        <v>1.4</v>
+        <v>1.29</v>
       </c>
       <c r="U113" s="212">
         <f>IF($A113="*","",IF(SRV_TH!U29=0,"",SRV_TH!U29))</f>
@@ -34523,14 +34518,14 @@
       </c>
       <c r="AL113" s="210"/>
       <c r="AM113" s="208">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN113" s="176"/>
       <c r="AO113" s="176"/>
       <c r="AP113" s="172"/>
       <c r="AQ113" s="45" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR113" s="45" t="str">
@@ -34538,25 +34533,25 @@
         <v>IE,National</v>
       </c>
       <c r="AS113" s="45" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SH-PU_HET_N1</v>
+      </c>
+      <c r="AT113" s="45" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Centralized DistrictH_Heat Exchanger_SH-WH</v>
+      </c>
+      <c r="AU113" s="45" t="str">
         <f t="shared" si="41"/>
-        <v>S-SH-PU_HET_N1</v>
-      </c>
-      <c r="AT113" s="45" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Centralized DistrictH_Heat Exchanger_SH-WH</v>
-      </c>
-      <c r="AU113" s="45" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV113" s="45" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV113" s="45" t="str">
-        <f t="shared" si="43"/>
         <v>GW</v>
       </c>
       <c r="AW113" s="45"/>
       <c r="AX113" s="45"/>
       <c r="AY113" s="45" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>YES</v>
       </c>
     </row>
@@ -34612,7 +34607,7 @@
       <c r="AO114" s="211"/>
       <c r="AP114" s="172"/>
       <c r="AQ114" s="57" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>*Water Heat-only</v>
       </c>
       <c r="AR114" s="57" t="str">
@@ -34620,25 +34615,25 @@
         <v/>
       </c>
       <c r="AS114" s="57" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="AT114" s="57" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="AU114" s="57" t="str">
         <f t="shared" si="41"/>
         <v/>
       </c>
-      <c r="AT114" s="57" t="str">
-        <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="AU114" s="57" t="str">
+      <c r="AV114" s="57" t="str">
         <f t="shared" si="42"/>
-        <v/>
-      </c>
-      <c r="AV114" s="57" t="str">
-        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AW114" s="57"/>
       <c r="AX114" s="57"/>
       <c r="AY114" s="57" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
@@ -34774,14 +34769,14 @@
       </c>
       <c r="AL115" s="84"/>
       <c r="AM115" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN115" s="211"/>
       <c r="AO115" s="211"/>
       <c r="AP115" s="172"/>
       <c r="AQ115" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR115" s="42" t="str">
@@ -34789,23 +34784,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS115" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-WH-PU_ELC_N1</v>
+      </c>
+      <c r="AT115" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Electric water heater_WH</v>
+      </c>
+      <c r="AU115" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-WH-PU_ELC_N1</v>
-      </c>
-      <c r="AT115" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Electric water heater_WH</v>
-      </c>
-      <c r="AU115" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV115" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV115" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY115" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY115" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -34941,14 +34936,14 @@
       </c>
       <c r="AL116" s="40"/>
       <c r="AM116" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN116" s="211"/>
       <c r="AO116" s="211"/>
       <c r="AP116" s="172"/>
       <c r="AQ116" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR116" s="42" t="str">
@@ -34956,23 +34951,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS116" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-WH-PU_SOL_N1</v>
+      </c>
+      <c r="AT116" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Solar water heater_WH</v>
+      </c>
+      <c r="AU116" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-WH-PU_SOL_N1</v>
-      </c>
-      <c r="AT116" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Solar water heater_WH</v>
-      </c>
-      <c r="AU116" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV116" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV116" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY116" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY116" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -35108,14 +35103,14 @@
       </c>
       <c r="AL117" s="84"/>
       <c r="AM117" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN117" s="172"/>
       <c r="AO117" s="172"/>
       <c r="AP117" s="172"/>
       <c r="AQ117" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR117" s="42" t="str">
@@ -35123,23 +35118,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS117" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-WH-PU_GAS_N1</v>
+      </c>
+      <c r="AT117" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Gas water heater_WH</v>
+      </c>
+      <c r="AU117" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-WH-PU_GAS_N1</v>
-      </c>
-      <c r="AT117" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Gas water heater_WH</v>
-      </c>
-      <c r="AU117" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV117" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV117" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY117" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY117" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -35270,19 +35265,19 @@
         <v/>
       </c>
       <c r="AK118" s="68">
-        <f t="shared" ref="AK118:AK119" si="51">IF($A118="*","",31.536)</f>
+        <f t="shared" ref="AK118:AK119" si="50">IF($A118="*","",31.536)</f>
         <v>31.536000000000001</v>
       </c>
       <c r="AL118" s="84"/>
       <c r="AM118" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN118" s="172"/>
       <c r="AO118" s="172"/>
       <c r="AP118" s="172"/>
       <c r="AQ118" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR118" s="42" t="str">
@@ -35290,23 +35285,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS118" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-WH-PU_BIO_N1</v>
+      </c>
+      <c r="AT118" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Biomass water heater_WH</v>
+      </c>
+      <c r="AU118" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-WH-PU_BIO_N1</v>
-      </c>
-      <c r="AT118" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Biomass water heater_WH</v>
-      </c>
-      <c r="AU118" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV118" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV118" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY118" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY118" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -35438,19 +35433,19 @@
         <v/>
       </c>
       <c r="AK119" s="214">
-        <f t="shared" si="51"/>
+        <f t="shared" si="50"/>
         <v>31.536000000000001</v>
       </c>
       <c r="AL119" s="71"/>
       <c r="AM119" s="208">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN119" s="211"/>
       <c r="AO119" s="211"/>
       <c r="AP119" s="172"/>
       <c r="AQ119" s="45" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR119" s="45" t="str">
@@ -35458,25 +35453,25 @@
         <v>IE,National</v>
       </c>
       <c r="AS119" s="45" t="str">
+        <f t="shared" si="40"/>
+        <v>S-WH-PU_LPG_N1</v>
+      </c>
+      <c r="AT119" s="45" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - LPG water heater_WH</v>
+      </c>
+      <c r="AU119" s="45" t="str">
         <f t="shared" si="41"/>
-        <v>S-WH-PU_LPG_N1</v>
-      </c>
-      <c r="AT119" s="45" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - LPG water heater_WH</v>
-      </c>
-      <c r="AU119" s="45" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV119" s="45" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV119" s="45" t="str">
-        <f t="shared" si="43"/>
         <v>GW</v>
       </c>
       <c r="AW119" s="45"/>
       <c r="AX119" s="45"/>
       <c r="AY119" s="45" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>YES</v>
       </c>
     </row>
@@ -35532,7 +35527,7 @@
       <c r="AO120" s="211"/>
       <c r="AP120" s="172"/>
       <c r="AQ120" s="57" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>*Cooling-only</v>
       </c>
       <c r="AR120" s="57" t="str">
@@ -35540,25 +35535,25 @@
         <v/>
       </c>
       <c r="AS120" s="57" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="AT120" s="57" t="str">
+        <f t="shared" si="40"/>
+        <v/>
+      </c>
+      <c r="AU120" s="57" t="str">
         <f t="shared" si="41"/>
         <v/>
       </c>
-      <c r="AT120" s="57" t="str">
-        <f t="shared" si="41"/>
-        <v/>
-      </c>
-      <c r="AU120" s="57" t="str">
+      <c r="AV120" s="57" t="str">
         <f t="shared" si="42"/>
-        <v/>
-      </c>
-      <c r="AV120" s="57" t="str">
-        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="AW120" s="57"/>
       <c r="AX120" s="57"/>
       <c r="AY120" s="57" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
@@ -35694,14 +35689,14 @@
       </c>
       <c r="AL121" s="84"/>
       <c r="AM121" s="81">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN121" s="172"/>
       <c r="AO121" s="172"/>
       <c r="AP121" s="172"/>
       <c r="AQ121" s="42" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>PRE</v>
       </c>
       <c r="AR121" s="42" t="str">
@@ -35709,23 +35704,23 @@
         <v>IE,National</v>
       </c>
       <c r="AS121" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>S-SC-PU_ELC_N1</v>
+      </c>
+      <c r="AT121" s="42" t="str">
+        <f t="shared" si="40"/>
+        <v>Public Services - Room air conditioning Air-to-Air_SC</v>
+      </c>
+      <c r="AU121" s="42" t="str">
         <f t="shared" si="41"/>
-        <v>S-SC-PU_ELC_N1</v>
-      </c>
-      <c r="AT121" s="42" t="str">
-        <f t="shared" si="41"/>
-        <v>Public Services - Room air conditioning Air-to-Air_SC</v>
-      </c>
-      <c r="AU121" s="42" t="str">
+        <v>PJ</v>
+      </c>
+      <c r="AV121" s="42" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV121" s="42" t="str">
+        <v>GW</v>
+      </c>
+      <c r="AY121" s="42" t="str">
         <f t="shared" si="43"/>
-        <v>GW</v>
-      </c>
-      <c r="AY121" s="42" t="str">
-        <f t="shared" si="44"/>
         <v>YES</v>
       </c>
     </row>
@@ -35862,13 +35857,13 @@
       </c>
       <c r="AL122" s="71"/>
       <c r="AM122" s="208">
-        <f t="shared" si="46"/>
+        <f t="shared" si="45"/>
         <v>2019</v>
       </c>
       <c r="AN122" s="85"/>
       <c r="AO122" s="85"/>
       <c r="AQ122" s="45" t="str">
-        <f t="shared" ref="AQ122" si="52">IF(LEFT(A122)="*",A122,"PRE")</f>
+        <f t="shared" ref="AQ122" si="51">IF(LEFT(A122)="*",A122,"PRE")</f>
         <v>PRE</v>
       </c>
       <c r="AR122" s="45" t="str">
@@ -35876,25 +35871,25 @@
         <v>IE,National</v>
       </c>
       <c r="AS122" s="45" t="str">
-        <f t="shared" ref="AS122" si="53">IF(LEFT($A122)="*","",A122)</f>
+        <f t="shared" ref="AS122" si="52">IF(LEFT($A122)="*","",A122)</f>
         <v>S-SC-PU_ELC_N2</v>
       </c>
       <c r="AT122" s="45" t="str">
-        <f t="shared" ref="AT122" si="54">IF(LEFT($A122)="*","",B122)</f>
+        <f t="shared" ref="AT122" si="53">IF(LEFT($A122)="*","",B122)</f>
         <v>Public Services - Centralized air conditioning_SC</v>
       </c>
       <c r="AU122" s="45" t="str">
+        <f t="shared" si="41"/>
+        <v>PJ</v>
+      </c>
+      <c r="AV122" s="45" t="str">
         <f t="shared" si="42"/>
-        <v>PJ</v>
-      </c>
-      <c r="AV122" s="45" t="str">
-        <f t="shared" si="43"/>
         <v>GW</v>
       </c>
       <c r="AW122" s="45"/>
       <c r="AX122" s="45"/>
       <c r="AY122" s="45" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>YES</v>
       </c>
     </row>
@@ -56656,6 +56651,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -56668,11 +56668,6 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -56681,6 +56676,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101003D35AAEA1B2FCB4388BD96CEDC55F277" ma:contentTypeVersion="9" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="3dbe2424fad29e82dbed878f9c5e39b8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0e3883c7-7fd1-40f0-8067-c70ec1cfb7e8" xmlns:ns3="5976181e-0ba6-4027-87bb-22a58e318fb6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="13ef504368312e798a12ea4dafd4e8bd" ns2:_="" ns3:_="">
     <xsd:import namespace="0e3883c7-7fd1-40f0-8067-c70ec1cfb7e8"/>
@@ -56877,22 +56887,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA1E081D-67D2-4E7B-BE8D-7D1C1B8C3BE7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97068170-2C4B-42A9-8C54-B2D8E2BB2908}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BAA8BF1-CC80-4539-9D14-46D49F0014CE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -56909,21 +56921,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97068170-2C4B-42A9-8C54-B2D8E2BB2908}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA1E081D-67D2-4E7B-BE8D-7D1C1B8C3BE7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Reduce 2018 efficiency of heat exchanges in commercial services
..so that the same efficiency is applied throughout the modelling horizon.
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SRV_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_SRV_NewTechs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721B3F7F-AC28-4910-AD8E-F127499E129F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5F3E37-31DB-40CE-AA73-570A1A6C314B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="789" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13679,10 +13679,6 @@
     <xf numFmtId="0" fontId="54" fillId="7" borderId="0" xfId="117" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -13692,6 +13688,10 @@
     <xf numFmtId="0" fontId="26" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -18595,46 +18595,46 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="369" t="s">
+      <c r="A3" s="365" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="369" t="s">
+      <c r="B3" s="365" t="s">
         <v>159</v>
       </c>
-      <c r="C3" s="369" t="s">
+      <c r="C3" s="365" t="s">
         <v>160</v>
       </c>
-      <c r="D3" s="371" t="s">
+      <c r="D3" s="367" t="s">
         <v>161</v>
       </c>
-      <c r="E3" s="371"/>
-      <c r="F3" s="369" t="s">
+      <c r="E3" s="367"/>
+      <c r="F3" s="365" t="s">
         <v>162</v>
       </c>
-      <c r="G3" s="369" t="s">
+      <c r="G3" s="365" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="369" t="s">
+      <c r="H3" s="365" t="s">
         <v>163</v>
       </c>
-      <c r="I3" s="369" t="s">
+      <c r="I3" s="365" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="370"/>
-      <c r="B4" s="370"/>
-      <c r="C4" s="370"/>
+      <c r="A4" s="366"/>
+      <c r="B4" s="366"/>
+      <c r="C4" s="366"/>
       <c r="D4" s="59" t="s">
         <v>165</v>
       </c>
       <c r="E4" s="59" t="s">
         <v>166</v>
       </c>
-      <c r="F4" s="370"/>
-      <c r="G4" s="370"/>
-      <c r="H4" s="370"/>
-      <c r="I4" s="370"/>
+      <c r="F4" s="366"/>
+      <c r="G4" s="366"/>
+      <c r="H4" s="366"/>
+      <c r="I4" s="366"/>
     </row>
     <row r="5" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
@@ -18720,18 +18720,18 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="162"/>
-      <c r="B11" s="365" t="str">
+      <c r="B11" s="368" t="str">
         <f>"Data summary table with data from "&amp;A5</f>
         <v>Data summary table with data from S1</v>
       </c>
-      <c r="C11" s="366"/>
+      <c r="C11" s="369"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="27"/>
-      <c r="B12" s="367" t="s">
+      <c r="B12" s="370" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="368"/>
+      <c r="C12" s="371"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
@@ -19100,16 +19100,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="G3:G4"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="G3:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -19890,11 +19890,11 @@
   <dimension ref="A1:AY122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="AG69" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B21" sqref="B21"/>
       <selection pane="topRight" activeCell="B21" sqref="B21"/>
       <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
-      <selection pane="bottomRight" activeCell="AR87" sqref="AR87"/>
+      <selection pane="bottomRight" activeCell="I77" sqref="I77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28182,7 +28182,8 @@
         <v>SRVSH-CS, SRVWH-CS</v>
       </c>
       <c r="F72" s="215">
-        <v>1.4</v>
+        <f>IF($A72="*","",IF(SRV_TH!F29=0,"",SRV_TH!F29))</f>
+        <v>1.29</v>
       </c>
       <c r="G72" s="215">
         <f>IF($A72="*","",IF(SRV_TH!G29=0,"",SRV_TH!G29))</f>
@@ -53480,6 +53481,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -53492,11 +53498,6 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -53702,18 +53703,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -53736,18 +53737,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97068170-2C4B-42A9-8C54-B2D8E2BB2908}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA1E081D-67D2-4E7B-BE8D-7D1C1B8C3BE7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97068170-2C4B-42A9-8C54-B2D8E2BB2908}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Linking Services and RSD DH
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_SRV_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_SRV_NewTechs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5F3E37-31DB-40CE-AA73-570A1A6C314B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4687B456-14D7-408E-8594-352BACD06D88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="789" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="789" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="78" r:id="rId1"/>
@@ -13679,6 +13679,10 @@
     <xf numFmtId="0" fontId="54" fillId="7" borderId="0" xfId="117" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -13688,10 +13692,6 @@
     <xf numFmtId="0" fontId="26" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -18595,46 +18595,46 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="365" t="s">
+      <c r="A3" s="369" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="365" t="s">
+      <c r="B3" s="369" t="s">
         <v>159</v>
       </c>
-      <c r="C3" s="365" t="s">
+      <c r="C3" s="369" t="s">
         <v>160</v>
       </c>
-      <c r="D3" s="367" t="s">
+      <c r="D3" s="371" t="s">
         <v>161</v>
       </c>
-      <c r="E3" s="367"/>
-      <c r="F3" s="365" t="s">
+      <c r="E3" s="371"/>
+      <c r="F3" s="369" t="s">
         <v>162</v>
       </c>
-      <c r="G3" s="365" t="s">
+      <c r="G3" s="369" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="365" t="s">
+      <c r="H3" s="369" t="s">
         <v>163</v>
       </c>
-      <c r="I3" s="365" t="s">
+      <c r="I3" s="369" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="366"/>
-      <c r="B4" s="366"/>
-      <c r="C4" s="366"/>
+      <c r="A4" s="370"/>
+      <c r="B4" s="370"/>
+      <c r="C4" s="370"/>
       <c r="D4" s="59" t="s">
         <v>165</v>
       </c>
       <c r="E4" s="59" t="s">
         <v>166</v>
       </c>
-      <c r="F4" s="366"/>
-      <c r="G4" s="366"/>
-      <c r="H4" s="366"/>
-      <c r="I4" s="366"/>
+      <c r="F4" s="370"/>
+      <c r="G4" s="370"/>
+      <c r="H4" s="370"/>
+      <c r="I4" s="370"/>
     </row>
     <row r="5" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
@@ -18720,18 +18720,18 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="162"/>
-      <c r="B11" s="368" t="str">
+      <c r="B11" s="365" t="str">
         <f>"Data summary table with data from "&amp;A5</f>
         <v>Data summary table with data from S1</v>
       </c>
-      <c r="C11" s="369"/>
+      <c r="C11" s="366"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="27"/>
-      <c r="B12" s="370" t="s">
+      <c r="B12" s="367" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="371"/>
+      <c r="C12" s="368"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
@@ -19100,16 +19100,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:F4"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="G3:G4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -19890,11 +19890,11 @@
   <dimension ref="A1:AY122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="R10" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B21" sqref="B21"/>
       <selection pane="topRight" activeCell="B21" sqref="B21"/>
       <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
-      <selection pane="bottomRight" activeCell="I77" sqref="I77"/>
+      <selection pane="bottomRight" activeCell="AF30" sqref="AF30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22926,16 +22926,19 @@
         <v>250</v>
       </c>
       <c r="AC29" s="292">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="AD29" s="292">
-        <v>189.2</v>
+        <f>AC29*0.945</f>
+        <v>37.799999999999997</v>
       </c>
       <c r="AE29" s="292">
-        <v>178.4</v>
+        <f>AC29*0.89</f>
+        <v>35.6</v>
       </c>
       <c r="AF29" s="292">
-        <v>168.5</v>
+        <f>AC29*0.845</f>
+        <v>33.799999999999997</v>
       </c>
       <c r="AG29" s="293">
         <f>'JRC data'!CG62</f>
@@ -28260,19 +28263,19 @@
       </c>
       <c r="AC72" s="34">
         <f>IF($A72="*","",IF(SRV_TH!AC29=0,"",SRV_TH!AC29))</f>
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="AD72" s="34">
         <f>IF($A72="*","",IF(SRV_TH!AD29=0,"",SRV_TH!AD29))</f>
-        <v>189.2</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="AE72" s="34">
         <f>IF($A72="*","",IF(SRV_TH!AE29=0,"",SRV_TH!AE29))</f>
-        <v>178.4</v>
+        <v>35.6</v>
       </c>
       <c r="AF72" s="34">
         <f>IF($A72="*","",IF(SRV_TH!AF29=0,"",SRV_TH!AF29))</f>
-        <v>168.5</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="AG72" s="38">
         <f>IF($A72="*","",IF(SRV_TH!AG29=0,"",SRV_TH!AG29))</f>
@@ -34096,19 +34099,19 @@
       </c>
       <c r="AC113" s="34">
         <f>IF($A113="*","",IF(SRV_TH!AC29=0,"",SRV_TH!AC29))</f>
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="AD113" s="34">
         <f>IF($A113="*","",IF(SRV_TH!AD29=0,"",SRV_TH!AD29))</f>
-        <v>189.2</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="AE113" s="34">
         <f>IF($A113="*","",IF(SRV_TH!AE29=0,"",SRV_TH!AE29))</f>
-        <v>178.4</v>
+        <v>35.6</v>
       </c>
       <c r="AF113" s="34">
         <f>IF($A113="*","",IF(SRV_TH!AF29=0,"",SRV_TH!AF29))</f>
-        <v>168.5</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="AG113" s="38">
         <f>IF($A113="*","",IF(SRV_TH!AG29=0,"",SRV_TH!AG29))</f>
@@ -53481,11 +53484,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="BL4:BP4"/>
-    <mergeCell ref="BQ4:BU4"/>
-    <mergeCell ref="BW4:CA4"/>
-    <mergeCell ref="CB4:CF4"/>
-    <mergeCell ref="CG4:CK4"/>
     <mergeCell ref="BG4:BK4"/>
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="I4:M4"/>
@@ -53498,6 +53496,11 @@
     <mergeCell ref="AR4:AV4"/>
     <mergeCell ref="AW4:BA4"/>
     <mergeCell ref="BB4:BF4"/>
+    <mergeCell ref="BL4:BP4"/>
+    <mergeCell ref="BQ4:BU4"/>
+    <mergeCell ref="BW4:CA4"/>
+    <mergeCell ref="CB4:CF4"/>
+    <mergeCell ref="CG4:CK4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -53506,6 +53509,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101003D35AAEA1B2FCB4388BD96CEDC55F277" ma:contentTypeVersion="9" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="3dbe2424fad29e82dbed878f9c5e39b8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0e3883c7-7fd1-40f0-8067-c70ec1cfb7e8" xmlns:ns3="5976181e-0ba6-4027-87bb-22a58e318fb6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="13ef504368312e798a12ea4dafd4e8bd" ns2:_="" ns3:_="">
     <xsd:import namespace="0e3883c7-7fd1-40f0-8067-c70ec1cfb7e8"/>
@@ -53702,12 +53711,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -53718,6 +53721,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA1E081D-67D2-4E7B-BE8D-7D1C1B8C3BE7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BAA8BF1-CC80-4539-9D14-46D49F0014CE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -53736,15 +53748,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA1E081D-67D2-4E7B-BE8D-7D1C1B8C3BE7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97068170-2C4B-42A9-8C54-B2D8E2BB2908}">
   <ds:schemaRefs>

</xml_diff>